<commit_message>
sekhar - changes made to salaries
</commit_message>
<xml_diff>
--- a/public/October-2014-bank_statement.xlsx
+++ b/public/October-2014-bank_statement.xlsx
@@ -14,11 +14,18 @@
     <numFmt numFmtId="100" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="101" formatCode="yyyy/mm/dd hh:mm:ss"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Arial"/>
       <sz val="11"/>
       <family val="1"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="15"/>
+      <family val="1"/>
+      <b val="true"/>
+      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,10 +56,13 @@
   <cellStyleXfs count="1">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="1" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="0" numFmtId="14" fontId="0" fillId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" numFmtId="0" fontId="1" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0"/>
@@ -67,69 +77,58 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.68988764044944"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="58.07022471910112"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="17.38988764044944"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="9.68988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="7.489887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Bank Details and Netpay of Employees</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="inlineStr">
         <is>
           <t>Account Number</t>
         </is>
       </c>
-      <c r="B1" s="0" t="inlineStr">
+      <c r="B2" s="0" t="inlineStr">
         <is>
           <t>Employee_name</t>
         </is>
       </c>
-      <c r="C1" s="0" t="inlineStr">
+      <c r="C2" s="0" t="inlineStr">
         <is>
           <t>Netpay</t>
         </is>
       </c>
-      <c r="D1" s="0" t="inlineStr">
+      <c r="D2" s="0" t="inlineStr">
         <is>
           <t>Month</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0" t="n">
+    <row r="3">
+      <c r="A3" s="0" t="n">
         <v>3214569877412589</v>
       </c>
-      <c r="B2" s="0" t="inlineStr">
+      <c r="B3" s="0" t="inlineStr">
         <is>
           <t>Sekhar Beri</t>
         </is>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>8701.46</v>
-      </c>
-      <c r="D2" s="0" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="n">
-        <v>1427854125478541</v>
-      </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>Priyanka Muddana</t>
-        </is>
-      </c>
       <c r="C3" s="0" t="n">
-        <v>9040.0</v>
+        <v>8700.73</v>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
@@ -139,15 +138,15 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="n">
-        <v>32154698714</v>
+        <v>1427854125478541</v>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>Pattabhi RamaRao Galidevara</t>
+          <t>Priyanka Muddana</t>
         </is>
       </c>
       <c r="C4" s="0" t="n">
-        <v>11000.0</v>
+        <v>9040.0</v>
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
@@ -155,8 +154,29 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>32154698714</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>Pattabhi RamaRao Galidevara</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>10000.0</v>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>October</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
   <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
   <pageSetup/>

</xml_diff>

<commit_message>
Balaraju - added payroll
</commit_message>
<xml_diff>
--- a/public/October-2014-bank_statement.xlsx
+++ b/public/October-2014-bank_statement.xlsx
@@ -14,18 +14,11 @@
     <numFmt numFmtId="100" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="101" formatCode="yyyy/mm/dd hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Arial"/>
       <sz val="11"/>
       <family val="1"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="15"/>
-      <family val="1"/>
-      <b val="true"/>
-      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="2">
@@ -56,13 +49,10 @@
   <cellStyleXfs count="1">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="1" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="0" numFmtId="14" fontId="0" fillId="0" xfId="0" applyNumberFormat="1"/>
-    <xf borderId="0" numFmtId="0" fontId="1" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0"/>
@@ -77,58 +67,71 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="58.07022471910112"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.38988764044944"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.08988764044944"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.18988764044944"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.68988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="7.489887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="0" t="inlineStr">
         <is>
-          <t>Bank Details and Netpay of Employees</t>
+          <t>Account Number</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>Employee_name</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>Netpay</t>
+        </is>
+      </c>
+      <c r="D1" s="0" t="inlineStr">
+        <is>
+          <t>Month</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>Account Number</t>
+          <t>banka121</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>Employee_name</t>
+          <t>Sekhar Beri</t>
         </is>
       </c>
-      <c r="C2" s="0" t="inlineStr">
-        <is>
-          <t>Netpay</t>
-        </is>
+      <c r="C2" s="0" t="n">
+        <v>25379.3</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>Month</t>
+          <t>October</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="n">
-        <v>3214569877412589</v>
+        <v>1234567890</v>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>Sekhar Beri</t>
+          <t>BalaRaju Vankala</t>
         </is>
       </c>
       <c r="C3" s="0" t="n">
-        <v>8700.73</v>
+        <v>833333000000000.0</v>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
@@ -136,47 +139,8 @@
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="0" t="n">
-        <v>1427854125478541</v>
-      </c>
-      <c r="B4" s="0" t="inlineStr">
-        <is>
-          <t>Priyanka Muddana</t>
-        </is>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>9040.0</v>
-      </c>
-      <c r="D4" s="0" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="n">
-        <v>32154698714</v>
-      </c>
-      <c r="B5" s="0" t="inlineStr">
-        <is>
-          <t>Pattabhi RamaRao Galidevara</t>
-        </is>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>10000.0</v>
-      </c>
-      <c r="D5" s="0" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
   <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
   <pageSetup/>

</xml_diff>

<commit_message>
sekhar - deleted unwanted data
</commit_message>
<xml_diff>
--- a/public/October-2014-bank_statement.xlsx
+++ b/public/October-2014-bank_statement.xlsx
@@ -14,18 +14,11 @@
     <numFmt numFmtId="100" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="101" formatCode="yyyy/mm/dd hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Arial"/>
       <sz val="11"/>
       <family val="1"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="15"/>
-      <family val="1"/>
-      <b val="true"/>
-      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="2">
@@ -56,13 +49,10 @@
   <cellStyleXfs count="1">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="1" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="0" numFmtId="14" fontId="0" fillId="0" xfId="0" applyNumberFormat="1"/>
-    <xf borderId="0" numFmtId="0" fontId="1" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0"/>
@@ -77,58 +67,69 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="58.07022471910112"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.68988764044944"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="17.38988764044944"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="9.68988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="7.489887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t>Bank Details and Netpay of Employees</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0" t="inlineStr">
+      <c r="A1" s="0" t="inlineStr">
         <is>
           <t>Account Number</t>
         </is>
       </c>
-      <c r="B2" s="0" t="inlineStr">
+      <c r="B1" s="0" t="inlineStr">
         <is>
           <t>Employee_name</t>
         </is>
       </c>
-      <c r="C2" s="0" t="inlineStr">
+      <c r="C1" s="0" t="inlineStr">
         <is>
           <t>Netpay</t>
         </is>
       </c>
-      <c r="D2" s="0" t="inlineStr">
+      <c r="D1" s="0" t="inlineStr">
         <is>
           <t>Month</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="0" t="n">
+    <row r="2">
+      <c r="A2" s="0" t="n">
         <v>3214569877412589</v>
       </c>
-      <c r="B3" s="0" t="inlineStr">
+      <c r="B2" s="0" t="inlineStr">
         <is>
           <t>Sekhar Beri</t>
         </is>
       </c>
+      <c r="C2" s="0" t="n">
+        <v>10000.0</v>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>October</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>1427854125478541</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Priyanka Muddana</t>
+        </is>
+      </c>
       <c r="C3" s="0" t="n">
-        <v>8700.73</v>
+        <v>8701.46</v>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
@@ -138,15 +139,15 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="n">
-        <v>1427854125478541</v>
+        <v>32154698714</v>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>Priyanka Muddana</t>
+          <t>Pattabhi RamaRao Galidevara</t>
         </is>
       </c>
       <c r="C4" s="0" t="n">
-        <v>9040.0</v>
+        <v>6440.0</v>
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
@@ -154,29 +155,8 @@
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="0" t="n">
-        <v>32154698714</v>
-      </c>
-      <c r="B5" s="0" t="inlineStr">
-        <is>
-          <t>Pattabhi RamaRao Galidevara</t>
-        </is>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>10000.0</v>
-      </c>
-      <c r="D5" s="0" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
   <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
   <pageSetup/>

</xml_diff>

<commit_message>
Priyanka - pdf formate
</commit_message>
<xml_diff>
--- a/public/October-2014-bank_statement.xlsx
+++ b/public/October-2014-bank_statement.xlsx
@@ -67,13 +67,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.08988764044944"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.18988764044944"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="15.18988764044944"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="9.68988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="7.489887640449439"/>
@@ -102,14 +102,16 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0"/>
+      <c r="A2" s="0" t="n">
+        <v>17249172304</v>
+      </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
           <t>Sekhar Beri</t>
         </is>
       </c>
       <c r="C2" s="0" t="n">
-        <v>9040.0</v>
+        <v>1304.86</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
@@ -118,14 +120,18 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0"/>
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>awetwetawe</t>
+        </is>
+      </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
           <t>BalaRaju Vankala</t>
         </is>
       </c>
       <c r="C3" s="0" t="n">
-        <v>10000.0</v>
+        <v>1449.85</v>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
@@ -141,25 +147,9 @@
         </is>
       </c>
       <c r="C4" s="0" t="n">
-        <v>8701.46</v>
+        <v>17057.4</v>
       </c>
       <c r="D4" s="0" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0"/>
-      <c r="B5" s="0" t="inlineStr">
-        <is>
-          <t>pattabhi ramarao</t>
-        </is>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>8701.44</v>
-      </c>
-      <c r="D5" s="0" t="inlineStr">
         <is>
           <t>October</t>
         </is>

</xml_diff>

<commit_message>
pattabhi added schedular por pay slip pdf  generation
</commit_message>
<xml_diff>
--- a/public/October-2014-bank_statement.xlsx
+++ b/public/October-2014-bank_statement.xlsx
@@ -67,13 +67,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.18988764044944"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.08988764044944"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="15.18988764044944"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="9.68988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="7.489887640449439"/>
@@ -102,54 +102,16 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0" t="n">
-        <v>17249172304</v>
-      </c>
+      <c r="A2" s="0"/>
       <c r="B2" s="0" t="inlineStr">
         <is>
           <t>Sekhar Beri</t>
         </is>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1304.86</v>
+        <v>10000.0</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="inlineStr">
-        <is>
-          <t>awetwetawe</t>
-        </is>
-      </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>BalaRaju Vankala</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>1449.85</v>
-      </c>
-      <c r="D3" s="0" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0"/>
-      <c r="B4" s="0" t="inlineStr">
-        <is>
-          <t>Priyanka Muddana</t>
-        </is>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>17057.4</v>
-      </c>
-      <c r="D4" s="0" t="inlineStr">
         <is>
           <t>October</t>
         </is>

</xml_diff>

<commit_message>
sekhar - changes made to views
</commit_message>
<xml_diff>
--- a/public/October-2014-bank_statement.xlsx
+++ b/public/October-2014-bank_statement.xlsx
@@ -67,15 +67,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.08988764044944"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.68988764044944"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="15.18988764044944"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.589887640449438"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="7.489887640449439"/>
   </cols>
   <sheetData>
@@ -103,35 +103,17 @@
     </row>
     <row r="2">
       <c r="A2" s="0" t="n">
-        <v>3214569874</v>
+        <v>3214569877896541</v>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>sekhar Beri</t>
+          <t>Sekhar Beri</t>
         </is>
       </c>
       <c r="C2" s="0" t="n">
-        <v>8698.55</v>
+        <v>9840.0</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="n">
-        <v>3215284678</v>
-      </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>Priyanka Muddana</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>9300.15</v>
-      </c>
-      <c r="D3" s="0" t="inlineStr">
         <is>
           <t>October</t>
         </is>

</xml_diff>

<commit_message>
sekhar - changes made salaries and payroll controller
</commit_message>
<xml_diff>
--- a/public/October-2014-bank_statement.xlsx
+++ b/public/October-2014-bank_statement.xlsx
@@ -103,7 +103,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0" t="n">
-        <v>3216549871234561</v>
+        <v>3214569873214569</v>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
@@ -111,7 +111,7 @@
         </is>
       </c>
       <c r="C2" s="0" t="n">
-        <v>9673.84</v>
+        <v>4951.46</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
@@ -121,7 +121,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="n">
-        <v>321456987</v>
+        <v>3216549873216549</v>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
@@ -129,7 +129,7 @@
         </is>
       </c>
       <c r="C3" s="0" t="n">
-        <v>8701.46</v>
+        <v>12252.4</v>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
BalaRaju - Working on Spec
</commit_message>
<xml_diff>
--- a/public/October-2014-bank_statement.xlsx
+++ b/public/October-2014-bank_statement.xlsx
@@ -67,13 +67,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.68988764044944"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.08988764044944"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="15.18988764044944"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="9.68988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="7.489887640449439"/>
@@ -102,36 +102,16 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0" t="n">
-        <v>3214569873214569</v>
-      </c>
+      <c r="A2" s="0"/>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>Sekhar Beri</t>
+          <t>Balaraju vankala</t>
         </is>
       </c>
       <c r="C2" s="0" t="n">
-        <v>4951.46</v>
+        <v>87004.6</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="n">
-        <v>3216549873216549</v>
-      </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>Priyanka Muddana</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>12252.4</v>
-      </c>
-      <c r="D3" s="0" t="inlineStr">
         <is>
           <t>October</t>
         </is>

</xml_diff>